<commit_message>
Added assembly instructions and updated frame BOM
</commit_message>
<xml_diff>
--- a/Documentation Source/source/BOMs/hardware bom.xlsx
+++ b/Documentation Source/source/BOMs/hardware bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Syringe/Documentation Source/source/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15868BE8-EB51-3348-8942-140399294F90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E07EE8-4EBD-F944-B9EC-A559B0768382}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24000" yWindow="13500" windowWidth="38400" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>link</t>
   </si>
@@ -166,9 +171,6 @@
     <t>https://www.omc-stepperonline.com/hybrid-stepper-motor/nema-17-bipolar-18deg-60ncm-85ozin-064a-10v-42x42x60mm-4-wires-17hs24-0644s.html?search=17hs24-0644s</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>Qty for # of pumps</t>
   </si>
   <si>
@@ -262,9 +264,6 @@
     <t>Flanged ball bearing</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Flanged LMF8UU slide bearing</t>
   </si>
   <si>
@@ -280,7 +279,13 @@
     <t>3501-0804-0350</t>
   </si>
   <si>
-    <t>`</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -536,7 +541,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>BOM!$L$25:$L$35</c:f>
+              <c:f>BOM!$L$4:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -578,7 +583,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>BOM!$N$25:$N$35</c:f>
+              <c:f>BOM!$N$4:$N$14</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1487,13 +1492,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1787,10 +1792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA42"/>
+  <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W38" sqref="W38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1840,10 +1845,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -1851,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="6">
         <v>31.84</v>
@@ -1864,16 +1869,16 @@
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
       <c r="I2" s="7">
-        <f>A2*BOM!$L$23</f>
+        <f>A2*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J2" s="7">
@@ -1881,9 +1886,28 @@
         <v>5</v>
       </c>
       <c r="K2" s="1">
-        <f>J2*C2/BOM!$L$23</f>
+        <f>J2*C2/BOM!$L$2</f>
         <v>31.839999999999996</v>
       </c>
+      <c r="L2" s="12">
+        <v>5</v>
+      </c>
+      <c r="M2" s="11">
+        <f>SUMPRODUCT(BOM!J2:J20,BOM!C2:C20)</f>
+        <v>573.77</v>
+      </c>
+      <c r="N2" s="11">
+        <f>M2/L2</f>
+        <v>114.75399999999999</v>
+      </c>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
@@ -1909,7 +1933,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="7">
-        <f>A3*BOM!$L$23</f>
+        <f>A3*BOM!$L$2</f>
         <v>10</v>
       </c>
       <c r="J3" s="7">
@@ -1917,16 +1941,24 @@
         <v>1</v>
       </c>
       <c r="K3" s="1">
-        <f>J3*C3/BOM!$L$23</f>
+        <f>J3*C3/BOM!$L$2</f>
         <v>2.1040000000000001</v>
       </c>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6">
         <v>7.97</v>
@@ -1936,16 +1968,16 @@
         <v>`7804K147 &lt;https://www.mcmaster.com/#7804K147&gt;`_</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
       <c r="I4" s="7">
-        <f>A4*BOM!$L$23</f>
+        <f>A4*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J4" s="7">
@@ -1953,16 +1985,34 @@
         <v>5</v>
       </c>
       <c r="K4" s="1">
-        <f>J4*C4/BOM!$L$23</f>
+        <f>J4*C4/BOM!$L$2</f>
         <v>7.9700000000000006</v>
       </c>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="11">
+        <v>235.84</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" ref="N4:N13" si="2">M4/L4</f>
+        <v>235.84</v>
+      </c>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="6">
         <v>4.4000000000000004</v>
@@ -1981,17 +2031,32 @@
         <v>100</v>
       </c>
       <c r="I5" s="7">
-        <f>A5*BOM!$L$23</f>
+        <f>A5*BOM!$L$2</f>
         <v>20</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" ref="J5:J20" si="2">ROUNDUP(I5/H5,0)</f>
+        <f t="shared" ref="J5:J20" si="3">ROUNDUP(I5/H5,0)</f>
         <v>1</v>
       </c>
       <c r="K5" s="1">
-        <f>J5*C5/BOM!$L$23</f>
+        <f>J5*C5/BOM!$L$2</f>
         <v>0.88000000000000012</v>
       </c>
+      <c r="L5" s="13">
+        <v>2</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -2017,24 +2082,39 @@
         <v>100</v>
       </c>
       <c r="I6" s="7">
-        <f>A6*BOM!$L$23</f>
+        <f>A6*BOM!$L$2</f>
         <v>20</v>
       </c>
       <c r="J6" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <f>J6*C6/BOM!$L$2</f>
+        <v>2</v>
+      </c>
+      <c r="L6" s="13">
+        <v>3</v>
+      </c>
+      <c r="N6" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
-        <f>J6*C6/BOM!$L$23</f>
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="6">
         <v>3.36</v>
@@ -2044,33 +2124,48 @@
         <v>`92005A130 &lt;https://www.mcmaster.com/#92005A130&gt;`_</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>100</v>
       </c>
       <c r="I7" s="7">
-        <f>A7*BOM!$L$23</f>
+        <f>A7*BOM!$L$2</f>
         <v>20</v>
       </c>
       <c r="J7" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <f>J7*C7/BOM!$L$2</f>
+        <v>0.67199999999999993</v>
+      </c>
+      <c r="L7" s="13">
+        <v>4</v>
+      </c>
+      <c r="N7" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K7" s="1">
-        <f>J7*C7/BOM!$L$23</f>
-        <v>0.67199999999999993</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="6">
         <v>3.88</v>
@@ -2080,33 +2175,51 @@
         <v>`92005A132 &lt;https://www.mcmaster.com/#92005A132&gt;`_</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H8" s="1">
         <v>100</v>
       </c>
       <c r="I8" s="7">
-        <f>A8*BOM!$L$23</f>
+        <f>A8*BOM!$L$2</f>
         <v>20</v>
       </c>
       <c r="J8" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <f>J8*C8/BOM!$L$2</f>
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="L8" s="13">
+        <v>5</v>
+      </c>
+      <c r="M8" s="11">
+        <v>625.77</v>
+      </c>
+      <c r="N8" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="1">
-        <f>J8*C8/BOM!$L$23</f>
-        <v>0.77600000000000002</v>
-      </c>
+        <v>125.154</v>
+      </c>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="6">
         <v>4.7</v>
@@ -2125,24 +2238,39 @@
         <v>100</v>
       </c>
       <c r="I9" s="7">
-        <f>A9*BOM!$L$23</f>
-        <v>70</v>
+        <f>A9*BOM!$L$2</f>
+        <v>80</v>
       </c>
       <c r="J9" s="7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
+        <f>J9*C9/BOM!$L$2</f>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="L9" s="13">
+        <v>6</v>
+      </c>
+      <c r="N9" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K9" s="1">
-        <f>J9*C9/BOM!$L$23</f>
-        <v>0.94000000000000006</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="6">
         <v>7.2</v>
@@ -2161,24 +2289,39 @@
         <v>50</v>
       </c>
       <c r="I10" s="7">
-        <f>A10*BOM!$L$23</f>
-        <v>50</v>
+        <f>A10*BOM!$L$2</f>
+        <v>100</v>
       </c>
       <c r="J10" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K10" s="1">
+        <f>J10*C10/BOM!$L$2</f>
+        <v>2.88</v>
+      </c>
+      <c r="L10" s="13">
+        <v>7</v>
+      </c>
+      <c r="N10" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K10" s="1">
-        <f>J10*C10/BOM!$L$23</f>
-        <v>1.44</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="6">
         <v>10.51</v>
@@ -2188,26 +2331,41 @@
         <v>`9657K267 &lt;https://www.mcmaster.com/#9657K267&gt;`_</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H11" s="1">
         <v>12</v>
       </c>
       <c r="I11" s="7">
-        <f>A11*BOM!$L$23</f>
+        <f>A11*BOM!$L$2</f>
         <v>20</v>
       </c>
       <c r="J11" s="7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <f>J11*C11/BOM!$L$2</f>
+        <v>4.2039999999999997</v>
+      </c>
+      <c r="L11" s="13">
+        <v>8</v>
+      </c>
+      <c r="N11" s="11">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K11" s="1">
-        <f>J11*C11/BOM!$L$23</f>
-        <v>4.2039999999999997</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -2233,28 +2391,43 @@
         <v>1</v>
       </c>
       <c r="I12" s="7">
-        <f>A12*BOM!$L$23</f>
+        <f>A12*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J12" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K12" s="1">
+        <f>J12*C12/BOM!$L$2</f>
+        <v>5.33</v>
+      </c>
+      <c r="L12" s="13">
+        <v>9</v>
+      </c>
+      <c r="N12" s="11">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="K12" s="1">
-        <f>J12*C12/BOM!$L$23</f>
-        <v>5.33</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
       <c r="X12" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
@@ -2262,20 +2435,20 @@
         <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" s="6">
         <v>7.99</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f t="shared" ref="D13:D17" si="3">CONCATENATE("`",F13," &lt;",G13,"&gt;`_")</f>
+        <f t="shared" ref="D13:D17" si="4">CONCATENATE("`",F13," &lt;",G13,"&gt;`_")</f>
         <v>`3501-0804-0350 &lt;https://www.servocity.com/lead-screws#371=448&gt;`_</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>22</v>
@@ -2284,19 +2457,37 @@
         <v>1</v>
       </c>
       <c r="I13" s="7">
-        <f>A13*BOM!$L$23</f>
+        <f>A13*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J13" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K13" s="1">
+        <f>J13*C13/BOM!$L$2</f>
+        <v>7.99</v>
+      </c>
+      <c r="L13" s="13">
+        <v>10</v>
+      </c>
+      <c r="M13" s="15">
+        <v>1115.8699999999999</v>
+      </c>
+      <c r="N13" s="11">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="K13" s="1">
-        <f>J13*C13/BOM!$L$23</f>
-        <v>7.99</v>
-      </c>
+        <v>111.58699999999999</v>
+      </c>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
       <c r="W13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="X13" s="1">
         <v>86.9</v>
@@ -2322,7 +2513,7 @@
         <v>7.99</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>`545315 &lt;https://www.servocity.com/8mm-4-start-hub&gt;`_</v>
       </c>
       <c r="F14" s="1">
@@ -2335,19 +2526,30 @@
         <v>1</v>
       </c>
       <c r="I14" s="7">
-        <f>A14*BOM!$L$23</f>
+        <f>A14*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="K14" s="1">
-        <f>J14*C14/BOM!$L$23</f>
+        <f>J14*C14/BOM!$L$2</f>
         <v>7.99</v>
       </c>
+      <c r="L14" s="13">
+        <v>11</v>
+      </c>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
       <c r="W14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X14" s="1">
         <v>105.3</v>
@@ -2373,7 +2575,7 @@
         <v>3.49</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>`634310 &lt;https://www.servocity.com/8mm-stainless-steel-precision-shafting#371=460&gt;`_</v>
       </c>
       <c r="F15" s="1">
@@ -2386,19 +2588,27 @@
         <v>1</v>
       </c>
       <c r="I15" s="7">
-        <f>A15*BOM!$L$23</f>
+        <f>A15*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J15" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="K15" s="1">
-        <f>J15*C15/BOM!$L$23</f>
+        <f>J15*C15/BOM!$L$2</f>
         <v>3.4900000000000007</v>
       </c>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
       <c r="W15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X15" s="10">
         <v>110.8</v>
@@ -2424,7 +2634,7 @@
         <v>7.99</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>`B01M287GNY &lt;https://www.amazon.com/RepRap-Champion-Coupler-Routers-printers/dp/B01M287GNY/ref=sr_1_12?ie=UTF8&amp;qid=1488495177&amp;sr=8-12&amp;keywords=5+to+8mm+coupler&gt;`_</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -2440,19 +2650,27 @@
         <v>2</v>
       </c>
       <c r="I16" s="7">
-        <f>A16*BOM!$L$23</f>
+        <f>A16*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="K16" s="1">
-        <f>J16*C16/BOM!$L$23</f>
+        <f>J16*C16/BOM!$L$2</f>
         <v>4.7939999999999996</v>
       </c>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
       <c r="W16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X16" s="1">
         <v>152.4</v>
@@ -2467,25 +2685,25 @@
         <v>28.51</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" s="6">
         <v>7.11</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>`B00NQ2H8YUF17 &lt;https://www.amazon.com/uxcell-LMF8UU-Inside-Flange-Bearing/d&gt;`_</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
@@ -2494,26 +2712,39 @@
         <v>1</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K17" s="1">
-        <f>J17*C17/BOM!$L$23</f>
+        <f>J17*C17/BOM!$L$2</f>
         <v>1.4220000000000002</v>
       </c>
+      <c r="L17" s="14"/>
+      <c r="N17" s="11">
+        <f>N4-N13</f>
+        <v>124.25300000000001</v>
+      </c>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="6">
         <v>14.31</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" ref="D18:D19" si="4">CONCATENATE("`",F18," &lt;",G18,"&gt;`_")</f>
+        <f t="shared" ref="D18:D19" si="5">CONCATENATE("`",F18," &lt;",G18,"&gt;`_")</f>
         <v>`SJ5746-0-ND &lt;https://www.digikey.com/product-detail/en/3m/SJ61A1/SJ5746-0-ND/1768456&gt;`_</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -2529,30 +2760,30 @@
         <v>144</v>
       </c>
       <c r="I18" s="7">
-        <f>A18*BOM!$L$23</f>
-        <v>20</v>
+        <f>A18*BOM!$L$2</f>
+        <v>40</v>
       </c>
       <c r="J18" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K18" s="1">
-        <f>J18*C18/BOM!$L$23</f>
+        <f>J18*C18/BOM!$L$2</f>
         <v>2.8620000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="6">
         <v>4.1100000000000003</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>`255-5122-ND &lt;https://www.digikey.com/products/en?keywords=255-5122-nd&gt;`_</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -2565,24 +2796,24 @@
         <v>1</v>
       </c>
       <c r="I19" s="7">
-        <f>A19*BOM!$L$23</f>
+        <f>A19*BOM!$L$2</f>
         <v>10</v>
       </c>
       <c r="J19" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="K19" s="1">
-        <f>J19*C19/BOM!$L$23</f>
+        <f>J19*C19/BOM!$L$2</f>
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="6">
         <v>18.39</v>
@@ -2604,336 +2835,23 @@
         <v>1</v>
       </c>
       <c r="I20" s="7">
-        <f>A20*BOM!$L$23</f>
+        <f>A20*BOM!$L$2</f>
         <v>5</v>
       </c>
       <c r="J20" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="K20" s="1">
-        <f>J20*C20/BOM!$L$23</f>
+        <f>J20*C20/BOM!$L$2</f>
         <v>18.39</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L23" s="12">
-        <v>5</v>
-      </c>
-      <c r="M23" s="11">
-        <f>SUMPRODUCT(BOM!J2:J20,BOM!C2:C20)</f>
-        <v>566.56999999999994</v>
-      </c>
-      <c r="N23" s="11">
-        <f>M23/L23</f>
-        <v>113.31399999999999</v>
-      </c>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
-      <c r="R24"/>
-      <c r="S24"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L25" s="13">
-        <v>1</v>
-      </c>
-      <c r="M25" s="11">
-        <v>235.84</v>
-      </c>
-      <c r="N25" s="11">
-        <f t="shared" ref="N25:N34" si="5">M25/L25</f>
-        <v>235.84</v>
-      </c>
-      <c r="O25"/>
-      <c r="P25"/>
-      <c r="Q25"/>
-      <c r="R25"/>
-      <c r="S25"/>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L26" s="13">
-        <v>2</v>
-      </c>
-      <c r="N26" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
-      <c r="R26"/>
-      <c r="S26"/>
-      <c r="T26"/>
-      <c r="U26"/>
-      <c r="V26"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L27" s="13">
-        <v>3</v>
-      </c>
-      <c r="N27" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O27"/>
-      <c r="P27"/>
-      <c r="Q27"/>
-      <c r="R27"/>
-      <c r="S27"/>
-      <c r="T27"/>
-      <c r="U27"/>
-      <c r="V27"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L28" s="13">
-        <v>4</v>
-      </c>
-      <c r="N28" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O28"/>
-      <c r="P28"/>
-      <c r="Q28"/>
-      <c r="R28"/>
-      <c r="S28"/>
-      <c r="T28"/>
-      <c r="U28"/>
-      <c r="V28"/>
-      <c r="W28" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L29" s="13">
-        <v>5</v>
-      </c>
-      <c r="M29" s="11">
-        <v>625.77</v>
-      </c>
-      <c r="N29" s="11">
-        <f t="shared" si="5"/>
-        <v>125.154</v>
-      </c>
-      <c r="O29"/>
-      <c r="P29"/>
-      <c r="Q29"/>
-      <c r="R29"/>
-      <c r="S29"/>
-      <c r="T29"/>
-      <c r="U29"/>
-      <c r="V29"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L30" s="13">
-        <v>6</v>
-      </c>
-      <c r="N30" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O30"/>
-      <c r="P30"/>
-      <c r="Q30"/>
-      <c r="R30"/>
-      <c r="S30"/>
-      <c r="T30"/>
-      <c r="U30"/>
-      <c r="V30"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L31" s="13">
-        <v>7</v>
-      </c>
-      <c r="N31" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31"/>
-      <c r="S31"/>
-      <c r="T31"/>
-      <c r="U31"/>
-      <c r="V31"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="L32" s="13">
-        <v>8</v>
-      </c>
-      <c r="N32" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-    </row>
-    <row r="33" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L33" s="13">
-        <v>9</v>
-      </c>
-      <c r="N33" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-    </row>
-    <row r="34" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L34" s="13">
-        <v>10</v>
-      </c>
-      <c r="M34" s="15">
-        <v>1115.8699999999999</v>
-      </c>
-      <c r="N34" s="11">
-        <f t="shared" si="5"/>
-        <v>111.58699999999999</v>
-      </c>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-    </row>
-    <row r="35" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L35" s="13">
-        <v>11</v>
-      </c>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-    </row>
-    <row r="36" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-    </row>
-    <row r="37" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-    </row>
-    <row r="38" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L38" s="14"/>
-      <c r="N38" s="11">
-        <f>N25-N34</f>
-        <v>124.25300000000001</v>
-      </c>
-      <c r="O38"/>
-      <c r="P38"/>
-      <c r="Q38"/>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-    </row>
-    <row r="39" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-    </row>
-    <row r="40" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-    </row>
-    <row r="41" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-    </row>
-    <row r="42" spans="12:22" x14ac:dyDescent="0.2">
-      <c r="L42"/>
-      <c r="M42"/>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42"/>
-      <c r="Q42"/>
-      <c r="R42"/>
-      <c r="S42"/>
-      <c r="T42"/>
-      <c r="U42"/>
-      <c r="V42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A13:A15 A18:A19 A16" numberStoredAsText="1"/>
+    <ignoredError sqref="A13:A15 A19 A16" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Doc update and new licenses
</commit_message>
<xml_diff>
--- a/Documentation Source/source/BOMs/hardware bom.xlsx
+++ b/Documentation Source/source/BOMs/hardware bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Syringe/Documentation Source/source/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E68BA5-A1B1-CB45-9EB2-59C2F9294493}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FB7ED5-C2B7-DD42-9A0D-23FC124AF9A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -265,9 +267,6 @@
     <t>B00NQ2H8YUF17</t>
   </si>
   <si>
-    <t>https://www.amazon.com/uxcell-LMF8UU-Inside-Flange-Bearing/d</t>
-  </si>
-  <si>
     <t xml:space="preserve">350 x 8mm lead screw </t>
   </si>
   <si>
@@ -287,6 +286,9 @@
   </si>
   <si>
     <t>B07Q5Q3DCB</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=LMF8UU&amp;ref=nb_sb_noss_2</t>
   </si>
 </sst>
 </file>
@@ -2733,8 +2735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3160,7 +3162,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>67</v>
@@ -3213,7 +3215,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>68</v>
@@ -3387,7 +3389,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="6">
         <v>7.99</v>
@@ -3400,7 +3402,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>20</v>
@@ -3589,10 +3591,10 @@
         <v>27</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H16" s="1">
         <v>2</v>
@@ -3645,13 +3647,13 @@
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>`B00NQ2H8YUF17 &lt;https://www.amazon.com/uxcell-LMF8UU-Inside-Flange-Bearing/d&gt;`_</v>
+        <v>`B00NQ2H8YUF17 &lt;https://www.amazon.com/s?k=LMF8UU&amp;ref=nb_sb_noss_2&gt;`_</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>75</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
@@ -3683,7 +3685,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>69</v>

</xml_diff>